<commit_message>
second commit by saira
</commit_message>
<xml_diff>
--- a/public/assets/docs/report.xlsx
+++ b/public/assets/docs/report.xlsx
@@ -415,7 +415,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
@@ -434,6 +434,9 @@
     <col min="12" max="12" width="25.7109375" customWidth="1"/>
     <col min="13" max="13" width="25.7109375" customWidth="1"/>
     <col min="14" max="14" width="10.7109375" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" customWidth="1"/>
+    <col min="17" max="17" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -479,6 +482,15 @@
       <c r="N1" s="4" t="str">
         <v>Status</v>
       </c>
+      <c r="O1" s="4" t="str">
+        <v>Rating</v>
+      </c>
+      <c r="P1" s="4" t="str">
+        <v>Total Ratings</v>
+      </c>
+      <c r="Q1" s="4" t="str">
+        <v>Popularity</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="str">
@@ -520,6 +532,15 @@
       <c r="N2" s="2" t="str">
         <v>Active</v>
       </c>
+      <c r="O2" s="2" t="str">
+        <v>4</v>
+      </c>
+      <c r="P2" s="2" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="2" t="str">
+        <v>2</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="str">
@@ -561,6 +582,15 @@
       <c r="N3" s="2" t="str">
         <v>Active</v>
       </c>
+      <c r="O3" s="2" t="str">
+        <v>4</v>
+      </c>
+      <c r="P3" s="2" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="2" t="str">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="str">
@@ -602,6 +632,15 @@
       <c r="N4" s="2" t="str">
         <v>Active</v>
       </c>
+      <c r="O4" s="2" t="str">
+        <v>4</v>
+      </c>
+      <c r="P4" s="2" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="2" t="str">
+        <v>2</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="str">
@@ -643,6 +682,15 @@
       <c r="N5" s="2" t="str">
         <v>Active</v>
       </c>
+      <c r="O5" s="2" t="str">
+        <v>4.5</v>
+      </c>
+      <c r="P5" s="2" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="2" t="str">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="str">
@@ -684,6 +732,15 @@
       <c r="N6" s="2" t="str">
         <v>Active</v>
       </c>
+      <c r="O6" s="2" t="str">
+        <v>4.5</v>
+      </c>
+      <c r="P6" s="2" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="2" t="str">
+        <v>3</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="str">
@@ -725,6 +782,15 @@
       <c r="N7" s="2" t="str">
         <v>Active</v>
       </c>
+      <c r="O7" s="2" t="str">
+        <v>4</v>
+      </c>
+      <c r="P7" s="2" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="2" t="str">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="str">
@@ -766,22 +832,31 @@
       <c r="N8" s="2" t="str">
         <v>Active</v>
       </c>
-    </row>
-    <row r="9" xml:space="preserve">
+      <c r="O8" s="2" t="str">
+        <v>4.5</v>
+      </c>
+      <c r="P8" s="2" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="2" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
       <c r="A9" s="2" t="str">
-        <v>Biryani</v>
+        <v>veg</v>
       </c>
       <c r="B9" s="2" t="str">
-        <v>53d5ef71-935a-43dc-93ca-0d072f60d4f1</v>
+        <v>e70158bb-c576-4135-89f2-f007a943a58f</v>
       </c>
       <c r="C9" s="2" t="str">
-        <v>Hot Gulab Jamun</v>
+        <v>Mix Veg  Soup</v>
       </c>
       <c r="D9" s="2" t="str">
         <v>Veg</v>
       </c>
       <c r="E9" s="2" t="str">
-        <v>2 hours</v>
+        <v>15 min</v>
       </c>
       <c r="F9" s="2" t="str">
         <v>0</v>
@@ -795,76 +870,94 @@
       <c r="J9" s="2">
         <v>200</v>
       </c>
-      <c r="K9" s="2" t="str" xml:space="preserve">
+      <c r="K9" s="2" t="str">
+        <v>Soup is a primarily liquid food, generally served warm or hot, that is made by combining ingredients of meat or vegetables with stock, or water. Hot soups are additionally characterized by boiling solid ingredients in liquids in a pot until the flavors are extracted, forming a broth</v>
+      </c>
+      <c r="L9" s="2" t="str">
+        <v/>
+      </c>
+      <c r="M9" s="2" t="str">
+        <v>cutlery</v>
+      </c>
+      <c r="N9" s="2" t="str">
+        <v>Active</v>
+      </c>
+      <c r="O9" s="2" t="str">
+        <v>4</v>
+      </c>
+      <c r="P9" s="2" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="2" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" xml:space="preserve">
+      <c r="A10" s="2" t="str">
+        <v>Biryani</v>
+      </c>
+      <c r="B10" s="2" t="str">
+        <v>53d5ef71-935a-43dc-93ca-0d072f60d4f1</v>
+      </c>
+      <c r="C10" s="2" t="str">
+        <v>Hot Gulab Jamun</v>
+      </c>
+      <c r="D10" s="2" t="str">
+        <v>Veg</v>
+      </c>
+      <c r="E10" s="2" t="str">
+        <v>2 hours</v>
+      </c>
+      <c r="F10" s="2" t="str">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0</v>
+      </c>
+      <c r="H10" s="2" t="str">
+        <v/>
+      </c>
+      <c r="J10" s="2">
+        <v>200</v>
+      </c>
+      <c r="K10" s="2" t="str" xml:space="preserve">
         <v xml:space="preserve">Gulab Jamun is one of India’s most popular sweet. These deep-fried dumplings/donuts made of dried milk [khoya] are dipped in a rose-cardamom flavored sugar syrup and make quite a treat._x000d_
 In India, you would find gulab jamun at every wedding, party, birthday and festivals. In short if you arrange any Indian party and plan to keep only one dessert, chances are it will be gulab jamun!</v>
       </c>
-      <c r="L9" s="2" t="str">
+      <c r="L10" s="2" t="str">
         <v>Flavours</v>
       </c>
-      <c r="M9" s="2" t="str">
+      <c r="M10" s="2" t="str">
         <v>Packing Wraps</v>
       </c>
-      <c r="N9" s="2" t="str">
-        <v>Active</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="str">
-        <v>non-veg</v>
-      </c>
-      <c r="B10" s="2" t="str">
-        <v>83d29148-cfab-4cac-8259-e0403f2291fe</v>
-      </c>
-      <c r="C10" s="2" t="str">
-        <v>clear soup</v>
-      </c>
-      <c r="D10" s="2" t="str">
-        <v>Veg</v>
-      </c>
-      <c r="E10" s="2" t="str">
-        <v>15 min</v>
-      </c>
-      <c r="F10" s="2" t="str">
-        <v>0</v>
-      </c>
-      <c r="G10" s="2">
-        <v>0</v>
-      </c>
-      <c r="H10" s="2" t="str">
-        <v/>
-      </c>
-      <c r="J10" s="2">
-        <v>230</v>
-      </c>
-      <c r="K10" s="2" t="str">
-        <v>Soup is a primarily liquid food, generally served warm or hot, that is made by combining ingredients of meat or vegetables with stock, or water. Hot soups are additionally characterized by boiling solid ingredients in liquids in a pot until the flavors are extracted, forming a broth</v>
-      </c>
-      <c r="L10" s="2" t="str">
-        <v>ketchup pouch</v>
-      </c>
-      <c r="M10" s="2" t="str">
-        <v/>
-      </c>
       <c r="N10" s="2" t="str">
         <v>Active</v>
+      </c>
+      <c r="O10" s="2" t="str">
+        <v>4</v>
+      </c>
+      <c r="P10" s="2" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="2" t="str">
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="str">
-        <v>Biryani</v>
+        <v>non-veg</v>
       </c>
       <c r="B11" s="2" t="str">
-        <v>53d5ef71-935a-43dc-93ca-0d072f60d4f1</v>
+        <v>83d29148-cfab-4cac-8259-e0403f2291fe</v>
       </c>
       <c r="C11" s="2" t="str">
-        <v>Pakodas</v>
+        <v>clear soup</v>
       </c>
       <c r="D11" s="2" t="str">
         <v>Veg</v>
       </c>
       <c r="E11" s="2" t="str">
-        <v>30 Minuts</v>
+        <v>15 min</v>
       </c>
       <c r="F11" s="2" t="str">
         <v>0</v>
@@ -876,19 +969,28 @@
         <v/>
       </c>
       <c r="J11" s="2">
-        <v>100</v>
+        <v>230</v>
       </c>
       <c r="K11" s="2" t="str">
-        <v>Pakora, also called pikora, pakoda, pakodi, fakkura, bhajiya, bhajji, bhaji or ponako, is a fried snack, originating from the Indian subcontinent. It is a popular snack across the Indian subcontinent, where it is served in restaurants and sold by street vendors</v>
+        <v>Soup is a primarily liquid food, generally served warm or hot, that is made by combining ingredients of meat or vegetables with stock, or water. Hot soups are additionally characterized by boiling solid ingredients in liquids in a pot until the flavors are extracted, forming a broth</v>
       </c>
       <c r="L11" s="2" t="str">
-        <v/>
+        <v>ketchup pouch</v>
       </c>
       <c r="M11" s="2" t="str">
         <v/>
       </c>
       <c r="N11" s="2" t="str">
         <v>Active</v>
+      </c>
+      <c r="O11" s="2" t="str">
+        <v>4</v>
+      </c>
+      <c r="P11" s="2" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="2" t="str">
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -899,7 +1001,7 @@
         <v>53d5ef71-935a-43dc-93ca-0d072f60d4f1</v>
       </c>
       <c r="C12" s="2" t="str">
-        <v>Paneer Samosa</v>
+        <v>Pakodas</v>
       </c>
       <c r="D12" s="2" t="str">
         <v>Veg</v>
@@ -917,39 +1019,48 @@
         <v/>
       </c>
       <c r="J12" s="2">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="K12" s="2" t="str">
-        <v>Fried or baked pastry with a savoury filling, such as spiced potatoes, onions, peas, cheese, beef and other meats, or lentils. It may take different forms, including triangular, cone, or half-moon shapes, depending on the region.[2][3][4] The Indian style, often accompanied by a chutney, is probably the most widely known of a broad family of recipes from Africa to China, which have origins in medieval times or earlier.[2] Samosas are a popular entrée, appetizer, or snack in the local cuisines of the Indian subcontinent, Western Asia, Southeast Asia, the Mediterranean, and Africa. Due to emigration and cultural diffusion from these areas, samosas today are often prepared in other regions.</v>
+        <v>Pakora, also called pikora, pakoda, pakodi, fakkura, bhajiya, bhajji, bhaji or ponako, is a fried snack, originating from the Indian subcontinent. It is a popular snack across the Indian subcontinent, where it is served in restaurants and sold by street vendors</v>
       </c>
       <c r="L12" s="2" t="str">
-        <v>Salads,Chutney,Red-Peppar</v>
+        <v/>
       </c>
       <c r="M12" s="2" t="str">
-        <v>Packing Wraps</v>
+        <v/>
       </c>
       <c r="N12" s="2" t="str">
         <v>Active</v>
+      </c>
+      <c r="O12" s="2" t="str">
+        <v>4</v>
+      </c>
+      <c r="P12" s="2" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="2" t="str">
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="str">
-        <v>veg</v>
+        <v>Soups</v>
       </c>
       <c r="B13" s="2" t="str">
-        <v>e70158bb-c576-4135-89f2-f007a943a58f</v>
+        <v>aa7b0190-97b1-4519-bf66-df04f5f33b85</v>
       </c>
       <c r="C13" s="2" t="str">
-        <v>Sweet Corn Soup</v>
+        <v>chicken Sour</v>
       </c>
       <c r="D13" s="2" t="str">
-        <v>Veg</v>
+        <v>Non-Veg</v>
       </c>
       <c r="E13" s="2" t="str">
-        <v>15 min</v>
+        <v>20 min</v>
       </c>
       <c r="F13" s="2" t="str">
-        <v>0</v>
+        <v>260</v>
       </c>
       <c r="G13" s="2">
         <v>0</v>
@@ -958,19 +1069,125 @@
         <v/>
       </c>
       <c r="J13" s="2">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="K13" s="2" t="str">
         <v>Soup is a primarily liquid food, generally served warm or hot, that is made by combining ingredients of meat or vegetables with stock, or water. Hot soups are additionally characterized by boiling solid ingredients in liquids in a pot until the flavors are extracted, forming a broth</v>
       </c>
       <c r="L13" s="2" t="str">
+        <v/>
+      </c>
+      <c r="N13" s="2" t="str">
+        <v>Active</v>
+      </c>
+      <c r="O13" s="2" t="str">
+        <v>0</v>
+      </c>
+      <c r="P13" s="2" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="2" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="str">
+        <v>Biryani</v>
+      </c>
+      <c r="B14" s="2" t="str">
+        <v>53d5ef71-935a-43dc-93ca-0d072f60d4f1</v>
+      </c>
+      <c r="C14" s="2" t="str">
+        <v>Paneer Samosa</v>
+      </c>
+      <c r="D14" s="2" t="str">
+        <v>Veg</v>
+      </c>
+      <c r="E14" s="2" t="str">
+        <v>30 Minuts</v>
+      </c>
+      <c r="F14" s="2" t="str">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2" t="str">
+        <v/>
+      </c>
+      <c r="J14" s="2">
+        <v>50</v>
+      </c>
+      <c r="K14" s="2" t="str">
+        <v>Fried or baked pastry with a savoury filling, such as spiced potatoes, onions, peas, cheese, beef and other meats, or lentils. It may take different forms, including triangular, cone, or half-moon shapes, depending on the region.[2][3][4] The Indian style, often accompanied by a chutney, is probably the most widely known of a broad family of recipes from Africa to China, which have origins in medieval times or earlier.[2] Samosas are a popular entrée, appetizer, or snack in the local cuisines of the Indian subcontinent, Western Asia, Southeast Asia, the Mediterranean, and Africa. Due to emigration and cultural diffusion from these areas, samosas today are often prepared in other regions.</v>
+      </c>
+      <c r="L14" s="2" t="str">
+        <v>Salads,Chutney,Red-Peppar</v>
+      </c>
+      <c r="M14" s="2" t="str">
+        <v>Packing Wraps</v>
+      </c>
+      <c r="N14" s="2" t="str">
+        <v>Active</v>
+      </c>
+      <c r="O14" s="2" t="str">
+        <v>4</v>
+      </c>
+      <c r="P14" s="2" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="2" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="str">
+        <v>veg</v>
+      </c>
+      <c r="B15" s="2" t="str">
+        <v>e70158bb-c576-4135-89f2-f007a943a58f</v>
+      </c>
+      <c r="C15" s="2" t="str">
+        <v>Sweet Corn Soup</v>
+      </c>
+      <c r="D15" s="2" t="str">
+        <v>Veg</v>
+      </c>
+      <c r="E15" s="2" t="str">
+        <v>15 min</v>
+      </c>
+      <c r="F15" s="2" t="str">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0</v>
+      </c>
+      <c r="H15" s="2" t="str">
+        <v/>
+      </c>
+      <c r="J15" s="2">
+        <v>200</v>
+      </c>
+      <c r="K15" s="2" t="str">
+        <v>Soup is a primarily liquid food, generally served warm or hot, that is made by combining ingredients of meat or vegetables with stock, or water. Hot soups are additionally characterized by boiling solid ingredients in liquids in a pot until the flavors are extracted, forming a broth</v>
+      </c>
+      <c r="L15" s="2" t="str">
         <v>ketchup pouch</v>
       </c>
-      <c r="M13" s="2" t="str">
+      <c r="M15" s="2" t="str">
         <v>cutlery</v>
       </c>
-      <c r="N13" s="2" t="str">
-        <v>Active</v>
+      <c r="N15" s="2" t="str">
+        <v>Active</v>
+      </c>
+      <c r="O15" s="2" t="str">
+        <v>4</v>
+      </c>
+      <c r="P15" s="2" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="2" t="str">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>